<commit_message>
Replaced comma with decimal.
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/digits_RP.xlsx
+++ b/raw-data-prep/raw_data/digits_RP.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Subno</t>
   </si>
@@ -46,9 +46,6 @@
   </si>
   <si>
     <t>Notes</t>
-  </si>
-  <si>
-    <t>919,1</t>
   </si>
   <si>
     <t>thumbs blocking fingers a little bit</t>
@@ -398,7 +395,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D19" sqref="D19"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -786,8 +783,8 @@
       <c r="G13">
         <v>87.19</v>
       </c>
-      <c r="H13" t="s">
-        <v>10</v>
+      <c r="H13">
+        <v>919.1</v>
       </c>
       <c r="I13">
         <v>82.87</v>
@@ -3055,7 +3052,7 @@
         <v>82.03</v>
       </c>
       <c r="J91" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="92" spans="1:10">
@@ -3261,7 +3258,7 @@
         <v>87.87</v>
       </c>
       <c r="J98" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="99" spans="1:10">
@@ -3757,7 +3754,7 @@
         <v>78.25</v>
       </c>
       <c r="J115" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="116" spans="1:10">
@@ -3992,7 +3989,7 @@
         <v>84.6</v>
       </c>
       <c r="J123" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="124" spans="1:10">

</xml_diff>

<commit_message>
Deleting obvious miscodes from digits_RP.xlsx
</commit_message>
<xml_diff>
--- a/raw-data-prep/raw_data/digits_RP.xlsx
+++ b/raw-data-prep/raw_data/digits_RP.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -11,6 +11,9 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$381</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
@@ -60,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -101,6 +104,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -149,7 +155,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -184,7 +190,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -393,11 +399,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:J381"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,7 +451,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>45</v>
       </c>
@@ -473,7 +480,7 @@
         <v>85.38</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>46</v>
       </c>
@@ -502,7 +509,7 @@
         <v>87.61</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>47</v>
       </c>
@@ -531,7 +538,7 @@
         <v>82.52</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>48</v>
       </c>
@@ -560,7 +567,7 @@
         <v>87.46</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>49</v>
       </c>
@@ -589,7 +596,7 @@
         <v>87.29</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>50</v>
       </c>
@@ -618,7 +625,7 @@
         <v>79.13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>51</v>
       </c>
@@ -647,7 +654,7 @@
         <v>81.59</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>52</v>
       </c>
@@ -676,7 +683,7 @@
         <v>86.79</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>53</v>
       </c>
@@ -705,7 +712,7 @@
         <v>81.23</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>54</v>
       </c>
@@ -734,7 +741,7 @@
         <v>83.79</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>55</v>
       </c>
@@ -763,7 +770,7 @@
         <v>89.02</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>56</v>
       </c>
@@ -792,7 +799,7 @@
         <v>82.87</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>57</v>
       </c>
@@ -821,7 +828,7 @@
         <v>89.68</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>58</v>
       </c>
@@ -850,7 +857,7 @@
         <v>85.62</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>59</v>
       </c>
@@ -879,7 +886,7 @@
         <v>89.35</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>60</v>
       </c>
@@ -908,7 +915,7 @@
         <v>87.72</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>61</v>
       </c>
@@ -937,7 +944,7 @@
         <v>81.89</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>62</v>
       </c>
@@ -966,7 +973,7 @@
         <v>86.01</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>63</v>
       </c>
@@ -995,7 +1002,7 @@
         <v>75.180000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>64</v>
       </c>
@@ -1024,7 +1031,7 @@
         <v>82.45</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>65</v>
       </c>
@@ -1053,7 +1060,7 @@
         <v>85.68</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>66</v>
       </c>
@@ -1082,7 +1089,7 @@
         <v>87.68</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>67</v>
       </c>
@@ -1111,7 +1118,7 @@
         <v>89.11</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>68</v>
       </c>
@@ -1140,7 +1147,7 @@
         <v>80.98</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>69</v>
       </c>
@@ -1169,7 +1176,7 @@
         <v>81.02</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>70</v>
       </c>
@@ -1198,7 +1205,7 @@
         <v>83.25</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>71</v>
       </c>
@@ -1227,7 +1234,7 @@
         <v>88.64</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>72</v>
       </c>
@@ -1256,7 +1263,7 @@
         <v>89.63</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>73</v>
       </c>
@@ -1285,7 +1292,7 @@
         <v>87.22</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>74</v>
       </c>
@@ -1314,7 +1321,7 @@
         <v>89.93</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>75</v>
       </c>
@@ -1343,7 +1350,7 @@
         <v>81.25</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>76</v>
       </c>
@@ -1372,7 +1379,7 @@
         <v>82.83</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>77</v>
       </c>
@@ -1382,9 +1389,6 @@
       <c r="C34">
         <v>84.26</v>
       </c>
-      <c r="D34">
-        <v>88.6</v>
-      </c>
       <c r="E34">
         <v>86.52</v>
       </c>
@@ -1401,7 +1405,7 @@
         <v>79.84</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>78</v>
       </c>
@@ -1430,7 +1434,7 @@
         <v>88.75</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>79</v>
       </c>
@@ -1459,7 +1463,7 @@
         <v>87.87</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>80</v>
       </c>
@@ -1488,7 +1492,7 @@
         <v>80.81</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>81</v>
       </c>
@@ -1517,7 +1521,7 @@
         <v>86.84</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>82</v>
       </c>
@@ -1546,7 +1550,7 @@
         <v>87.78</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>83</v>
       </c>
@@ -1591,20 +1595,14 @@
       <c r="E41">
         <v>84.18</v>
       </c>
-      <c r="F41">
-        <v>955</v>
-      </c>
       <c r="G41">
         <v>84.11</v>
       </c>
-      <c r="H41">
-        <v>686</v>
-      </c>
       <c r="I41">
         <v>81.790000000000006</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>85</v>
       </c>
@@ -1633,7 +1631,7 @@
         <v>85.33</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>86</v>
       </c>
@@ -1662,7 +1660,7 @@
         <v>89.38</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>87</v>
       </c>
@@ -1691,7 +1689,7 @@
         <v>88.78</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>88</v>
       </c>
@@ -1720,7 +1718,7 @@
         <v>86.82</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>89</v>
       </c>
@@ -1749,7 +1747,7 @@
         <v>86.47</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>90</v>
       </c>
@@ -1778,7 +1776,7 @@
         <v>88.89</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>91</v>
       </c>
@@ -1807,7 +1805,7 @@
         <v>89.1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>92</v>
       </c>
@@ -1836,7 +1834,7 @@
         <v>86.73</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>93</v>
       </c>
@@ -1865,7 +1863,7 @@
         <v>88.04</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>94</v>
       </c>
@@ -1894,7 +1892,7 @@
         <v>78.849999999999994</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>95</v>
       </c>
@@ -1923,7 +1921,7 @@
         <v>82.81</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>96</v>
       </c>
@@ -1952,7 +1950,7 @@
         <v>79.239999999999995</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>97</v>
       </c>
@@ -1981,7 +1979,7 @@
         <v>84.71</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>98</v>
       </c>
@@ -2010,7 +2008,7 @@
         <v>81.58</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>99</v>
       </c>
@@ -2039,7 +2037,7 @@
         <v>85.56</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>100</v>
       </c>
@@ -2068,7 +2066,7 @@
         <v>82.44</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>101</v>
       </c>
@@ -2097,7 +2095,7 @@
         <v>88.14</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>102</v>
       </c>
@@ -2126,7 +2124,7 @@
         <v>80.33</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>103</v>
       </c>
@@ -2155,7 +2153,7 @@
         <v>88.52</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>104</v>
       </c>
@@ -2184,7 +2182,7 @@
         <v>87.82</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>105</v>
       </c>
@@ -2213,7 +2211,7 @@
         <v>88.2</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>106</v>
       </c>
@@ -2242,7 +2240,7 @@
         <v>88.98</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>107</v>
       </c>
@@ -2271,7 +2269,7 @@
         <v>78.56</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>108</v>
       </c>
@@ -2300,7 +2298,7 @@
         <v>87.87</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>109</v>
       </c>
@@ -2329,7 +2327,7 @@
         <v>88.96</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>110</v>
       </c>
@@ -2358,7 +2356,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>111</v>
       </c>
@@ -2387,7 +2385,7 @@
         <v>85.19</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>112</v>
       </c>
@@ -2416,7 +2414,7 @@
         <v>85.08</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>113</v>
       </c>
@@ -2445,7 +2443,7 @@
         <v>82.69</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>114</v>
       </c>
@@ -2474,7 +2472,7 @@
         <v>87.52</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>115</v>
       </c>
@@ -2503,7 +2501,7 @@
         <v>83.98</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>116</v>
       </c>
@@ -2532,7 +2530,7 @@
         <v>80.38</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>117</v>
       </c>
@@ -2561,7 +2559,7 @@
         <v>84.93</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>118</v>
       </c>
@@ -2590,7 +2588,7 @@
         <v>81.819999999999993</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>119</v>
       </c>
@@ -2619,7 +2617,7 @@
         <v>87.32</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>120</v>
       </c>
@@ -2648,7 +2646,7 @@
         <v>87.07</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>121</v>
       </c>
@@ -2677,7 +2675,7 @@
         <v>84.74</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>122</v>
       </c>
@@ -2706,7 +2704,7 @@
         <v>86.05</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>123</v>
       </c>
@@ -2735,7 +2733,7 @@
         <v>87.91</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>124</v>
       </c>
@@ -2764,7 +2762,7 @@
         <v>88.2</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>125</v>
       </c>
@@ -2793,7 +2791,7 @@
         <v>81.099999999999994</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>126</v>
       </c>
@@ -2822,7 +2820,7 @@
         <v>88.44</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>127</v>
       </c>
@@ -2851,7 +2849,7 @@
         <v>89.5</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>128</v>
       </c>
@@ -2880,7 +2878,7 @@
         <v>84.65</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>129</v>
       </c>
@@ -2909,7 +2907,7 @@
         <v>84.63</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>130</v>
       </c>
@@ -2938,7 +2936,7 @@
         <v>82.3</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>131</v>
       </c>
@@ -2967,7 +2965,7 @@
         <v>89.94</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>132</v>
       </c>
@@ -2996,7 +2994,7 @@
         <v>85.88</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>133</v>
       </c>
@@ -3025,7 +3023,7 @@
         <v>81.13</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>134</v>
       </c>
@@ -3057,7 +3055,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>135</v>
       </c>
@@ -3086,7 +3084,7 @@
         <v>82.34</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>136</v>
       </c>
@@ -3115,7 +3113,7 @@
         <v>86.39</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>137</v>
       </c>
@@ -3144,7 +3142,7 @@
         <v>85.34</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>138</v>
       </c>
@@ -3173,7 +3171,7 @@
         <v>87.32</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>139</v>
       </c>
@@ -3202,7 +3200,7 @@
         <v>89.11</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>140</v>
       </c>
@@ -3231,7 +3229,7 @@
         <v>86.52</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>141</v>
       </c>
@@ -3263,7 +3261,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>142</v>
       </c>
@@ -3292,7 +3290,7 @@
         <v>86.62</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>143</v>
       </c>
@@ -3321,7 +3319,7 @@
         <v>89.44</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>144</v>
       </c>
@@ -3350,7 +3348,7 @@
         <v>80.400000000000006</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>145</v>
       </c>
@@ -3379,7 +3377,7 @@
         <v>81.069999999999993</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>146</v>
       </c>
@@ -3408,7 +3406,7 @@
         <v>88.56</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>147</v>
       </c>
@@ -3437,7 +3435,7 @@
         <v>87.25</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>148</v>
       </c>
@@ -3453,9 +3451,6 @@
       <c r="E105">
         <v>76.08</v>
       </c>
-      <c r="F105">
-        <v>88.7</v>
-      </c>
       <c r="G105">
         <v>79.56</v>
       </c>
@@ -3466,7 +3461,7 @@
         <v>88.17</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>149</v>
       </c>
@@ -3495,7 +3490,7 @@
         <v>81.96</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>150</v>
       </c>
@@ -3524,7 +3519,7 @@
         <v>87.66</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>151</v>
       </c>
@@ -3553,7 +3548,7 @@
         <v>86.08</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>152</v>
       </c>
@@ -3582,7 +3577,7 @@
         <v>89.88</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>153</v>
       </c>
@@ -3611,7 +3606,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>154</v>
       </c>
@@ -3640,7 +3635,7 @@
         <v>89.61</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>155</v>
       </c>
@@ -3669,7 +3664,7 @@
         <v>87.7</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>156</v>
       </c>
@@ -3698,7 +3693,7 @@
         <v>88.1</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>157</v>
       </c>
@@ -3727,7 +3722,7 @@
         <v>89.35</v>
       </c>
     </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>158</v>
       </c>
@@ -3759,7 +3754,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>159</v>
       </c>
@@ -3788,7 +3783,7 @@
         <v>88.4</v>
       </c>
     </row>
-    <row r="117" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>160</v>
       </c>
@@ -3817,7 +3812,7 @@
         <v>82.82</v>
       </c>
     </row>
-    <row r="118" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>161</v>
       </c>
@@ -3846,7 +3841,7 @@
         <v>85.62</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>162</v>
       </c>
@@ -3875,7 +3870,7 @@
         <v>84.11</v>
       </c>
     </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>163</v>
       </c>
@@ -3904,7 +3899,7 @@
         <v>84.31</v>
       </c>
     </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>164</v>
       </c>
@@ -3933,7 +3928,7 @@
         <v>81.63</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>165</v>
       </c>
@@ -3962,7 +3957,7 @@
         <v>85.24</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>166</v>
       </c>
@@ -3994,7 +3989,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>167</v>
       </c>
@@ -4023,7 +4018,7 @@
         <v>83.34</v>
       </c>
     </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>168</v>
       </c>
@@ -4052,7 +4047,7 @@
         <v>84.99</v>
       </c>
     </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>169</v>
       </c>
@@ -4081,7 +4076,7 @@
         <v>85.49</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>170</v>
       </c>
@@ -4110,7 +4105,7 @@
         <v>78.11</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>171</v>
       </c>
@@ -4139,7 +4134,7 @@
         <v>89.05</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>172</v>
       </c>
@@ -4168,7 +4163,7 @@
         <v>83.05</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>173</v>
       </c>
@@ -4197,7 +4192,7 @@
         <v>86.23</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>174</v>
       </c>
@@ -4226,7 +4221,7 @@
         <v>82.91</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>175</v>
       </c>
@@ -4255,7 +4250,7 @@
         <v>89.17</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>176</v>
       </c>
@@ -4284,7 +4279,7 @@
         <v>83.86</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>177</v>
       </c>
@@ -4313,7 +4308,7 @@
         <v>89.26</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>178</v>
       </c>
@@ -4342,7 +4337,7 @@
         <v>87.67</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>179</v>
       </c>
@@ -4371,7 +4366,7 @@
         <v>81.3</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>180</v>
       </c>
@@ -4400,7 +4395,7 @@
         <v>78.64</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>181</v>
       </c>
@@ -4429,7 +4424,7 @@
         <v>86.07</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>182</v>
       </c>
@@ -4458,7 +4453,7 @@
         <v>85.93</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>183</v>
       </c>
@@ -4516,7 +4511,7 @@
         <v>86.69</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>185</v>
       </c>
@@ -4545,7 +4540,7 @@
         <v>85.42</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>186</v>
       </c>
@@ -4574,7 +4569,7 @@
         <v>89.13</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>187</v>
       </c>
@@ -4603,7 +4598,7 @@
         <v>83.31</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>188</v>
       </c>
@@ -4632,7 +4627,7 @@
         <v>89.27</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>189</v>
       </c>
@@ -4661,7 +4656,7 @@
         <v>84.88</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>190</v>
       </c>
@@ -4690,7 +4685,7 @@
         <v>82.57</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>191</v>
       </c>
@@ -4719,7 +4714,7 @@
         <v>86.97</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>192</v>
       </c>
@@ -4748,7 +4743,7 @@
         <v>84.91</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>193</v>
       </c>
@@ -4777,7 +4772,7 @@
         <v>79.59</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>194</v>
       </c>
@@ -4806,7 +4801,7 @@
         <v>83.57</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>195</v>
       </c>
@@ -4835,7 +4830,7 @@
         <v>82.67</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>196</v>
       </c>
@@ -4864,7 +4859,7 @@
         <v>82.89</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>197</v>
       </c>
@@ -4893,7 +4888,7 @@
         <v>78.84</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>198</v>
       </c>
@@ -4922,7 +4917,7 @@
         <v>85.62</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>199</v>
       </c>
@@ -4951,7 +4946,7 @@
         <v>89.14</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>200</v>
       </c>
@@ -4980,7 +4975,7 @@
         <v>83.16</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>201</v>
       </c>
@@ -5009,7 +5004,7 @@
         <v>87.71</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>202</v>
       </c>
@@ -5038,7 +5033,7 @@
         <v>83.17</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>203</v>
       </c>
@@ -5067,7 +5062,7 @@
         <v>89.04</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>204</v>
       </c>
@@ -5096,7 +5091,7 @@
         <v>86.55</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>205</v>
       </c>
@@ -5125,7 +5120,7 @@
         <v>84.2</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>206</v>
       </c>
@@ -5154,7 +5149,7 @@
         <v>84.74</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>207</v>
       </c>
@@ -5183,7 +5178,7 @@
         <v>86.83</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>208</v>
       </c>
@@ -5212,7 +5207,7 @@
         <v>87.03</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>209</v>
       </c>
@@ -5241,7 +5236,7 @@
         <v>83.71</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>210</v>
       </c>
@@ -5270,7 +5265,7 @@
         <v>76.59</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>211</v>
       </c>
@@ -5299,7 +5294,7 @@
         <v>88.64</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>212</v>
       </c>
@@ -5328,7 +5323,7 @@
         <v>84.44</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>213</v>
       </c>
@@ -5357,7 +5352,7 @@
         <v>89.09</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>214</v>
       </c>
@@ -5386,7 +5381,7 @@
         <v>83.04</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>215</v>
       </c>
@@ -5415,7 +5410,7 @@
         <v>84.96</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>216</v>
       </c>
@@ -5444,7 +5439,7 @@
         <v>87.06</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>217</v>
       </c>
@@ -5473,7 +5468,7 @@
         <v>83.39</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>218</v>
       </c>
@@ -5502,7 +5497,7 @@
         <v>83.43</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>219</v>
       </c>
@@ -5531,7 +5526,7 @@
         <v>85.03</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>220</v>
       </c>
@@ -5560,7 +5555,7 @@
         <v>88.44</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>221</v>
       </c>
@@ -5589,7 +5584,7 @@
         <v>83.36</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>222</v>
       </c>
@@ -5618,7 +5613,7 @@
         <v>87.44</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>223</v>
       </c>
@@ -5647,7 +5642,7 @@
         <v>85.02</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>224</v>
       </c>
@@ -5676,7 +5671,7 @@
         <v>87.96</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>225</v>
       </c>
@@ -5705,7 +5700,7 @@
         <v>82.66</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>226</v>
       </c>
@@ -5734,7 +5729,7 @@
         <v>83.5</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>227</v>
       </c>
@@ -5763,7 +5758,7 @@
         <v>85.94</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>228</v>
       </c>
@@ -5792,7 +5787,7 @@
         <v>85.38</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>229</v>
       </c>
@@ -5821,7 +5816,7 @@
         <v>79.28</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>230</v>
       </c>
@@ -5850,7 +5845,7 @@
         <v>82.45</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>231</v>
       </c>
@@ -5879,7 +5874,7 @@
         <v>86.21</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>232</v>
       </c>
@@ -5908,7 +5903,7 @@
         <v>82.94</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>233</v>
       </c>
@@ -5937,7 +5932,7 @@
         <v>86.71</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>234</v>
       </c>
@@ -5966,7 +5961,7 @@
         <v>83.86</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>235</v>
       </c>
@@ -5995,7 +5990,7 @@
         <v>88.61</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>236</v>
       </c>
@@ -6024,7 +6019,7 @@
         <v>85.54</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>237</v>
       </c>
@@ -6053,7 +6048,7 @@
         <v>82.19</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>238</v>
       </c>
@@ -6082,7 +6077,7 @@
         <v>87.84</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>239</v>
       </c>
@@ -6111,7 +6106,7 @@
         <v>84.81</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>240</v>
       </c>
@@ -6140,7 +6135,7 @@
         <v>88.63</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>241</v>
       </c>
@@ -6169,7 +6164,7 @@
         <v>89.68</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>242</v>
       </c>
@@ -6198,7 +6193,7 @@
         <v>84.9</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>243</v>
       </c>
@@ -6227,7 +6222,7 @@
         <v>78.03</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>244</v>
       </c>
@@ -6256,7 +6251,7 @@
         <v>84.95</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>245</v>
       </c>
@@ -6285,7 +6280,7 @@
         <v>83.47</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>246</v>
       </c>
@@ -6314,7 +6309,7 @@
         <v>89.31</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>247</v>
       </c>
@@ -6343,7 +6338,7 @@
         <v>86.53</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>248</v>
       </c>
@@ -6372,7 +6367,7 @@
         <v>85.05</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>249</v>
       </c>
@@ -6401,7 +6396,7 @@
         <v>82.49</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>250</v>
       </c>
@@ -6430,7 +6425,7 @@
         <v>82.91</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>251</v>
       </c>
@@ -6459,7 +6454,7 @@
         <v>87.8</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>252</v>
       </c>
@@ -6488,7 +6483,7 @@
         <v>81.760000000000005</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>253</v>
       </c>
@@ -6517,7 +6512,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>254</v>
       </c>
@@ -6546,7 +6541,7 @@
         <v>88.37</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>255</v>
       </c>
@@ -6575,7 +6570,7 @@
         <v>89.22</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>256</v>
       </c>
@@ -6604,7 +6599,7 @@
         <v>88.01</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>257</v>
       </c>
@@ -6633,7 +6628,7 @@
         <v>87.49</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>258</v>
       </c>
@@ -6662,7 +6657,7 @@
         <v>87.34</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>259</v>
       </c>
@@ -6691,7 +6686,7 @@
         <v>87.91</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>260</v>
       </c>
@@ -6720,7 +6715,7 @@
         <v>87.44</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>261</v>
       </c>
@@ -6749,7 +6744,7 @@
         <v>88.83</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>262</v>
       </c>
@@ -6778,7 +6773,7 @@
         <v>89.94</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>263</v>
       </c>
@@ -6807,7 +6802,7 @@
         <v>88.59</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>264</v>
       </c>
@@ -6836,7 +6831,7 @@
         <v>85.96</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>265</v>
       </c>
@@ -6865,7 +6860,7 @@
         <v>88.97</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>266</v>
       </c>
@@ -6894,7 +6889,7 @@
         <v>89.77</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>267</v>
       </c>
@@ -6923,7 +6918,7 @@
         <v>85.95</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>268</v>
       </c>
@@ -6952,7 +6947,7 @@
         <v>84.1</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>269</v>
       </c>
@@ -6981,7 +6976,7 @@
         <v>81.61</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>270</v>
       </c>
@@ -7010,7 +7005,7 @@
         <v>88.49</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>271</v>
       </c>
@@ -7039,7 +7034,7 @@
         <v>78.180000000000007</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>272</v>
       </c>
@@ -7068,7 +7063,7 @@
         <v>85.19</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>273</v>
       </c>
@@ -7097,7 +7092,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>274</v>
       </c>
@@ -7126,7 +7121,7 @@
         <v>84.96</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>275</v>
       </c>
@@ -7155,7 +7150,7 @@
         <v>83.13</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>276</v>
       </c>
@@ -7184,7 +7179,7 @@
         <v>89.39</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>277</v>
       </c>
@@ -7213,7 +7208,7 @@
         <v>83.42</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>278</v>
       </c>
@@ -7242,7 +7237,7 @@
         <v>89.59</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>279</v>
       </c>
@@ -7271,7 +7266,7 @@
         <v>80.28</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>280</v>
       </c>
@@ -7300,7 +7295,7 @@
         <v>84.81</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>281</v>
       </c>
@@ -7329,7 +7324,7 @@
         <v>77.680000000000007</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>282</v>
       </c>
@@ -7358,7 +7353,7 @@
         <v>89.03</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>283</v>
       </c>
@@ -7416,7 +7411,7 @@
         <v>81.459999999999994</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>285</v>
       </c>
@@ -7445,7 +7440,7 @@
         <v>80.709999999999994</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>286</v>
       </c>
@@ -7474,7 +7469,7 @@
         <v>84.89</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>287</v>
       </c>
@@ -7503,7 +7498,7 @@
         <v>85.66</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>288</v>
       </c>
@@ -7532,7 +7527,7 @@
         <v>89.69</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>289</v>
       </c>
@@ -7561,7 +7556,7 @@
         <v>84.54</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>290</v>
       </c>
@@ -7590,7 +7585,7 @@
         <v>86.26</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>291</v>
       </c>
@@ -7619,7 +7614,7 @@
         <v>86.76</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>292</v>
       </c>
@@ -7648,7 +7643,7 @@
         <v>89.18</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>293</v>
       </c>
@@ -7677,7 +7672,7 @@
         <v>82.05</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>294</v>
       </c>
@@ -7706,7 +7701,7 @@
         <v>88.02</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>295</v>
       </c>
@@ -7735,7 +7730,7 @@
         <v>77.900000000000006</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>296</v>
       </c>
@@ -7764,7 +7759,7 @@
         <v>81.8</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>297</v>
       </c>
@@ -7793,7 +7788,7 @@
         <v>86.42</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>298</v>
       </c>
@@ -7822,7 +7817,7 @@
         <v>84.3</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>299</v>
       </c>
@@ -7851,7 +7846,7 @@
         <v>85.36</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="257" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>300</v>
       </c>
@@ -7880,7 +7875,7 @@
         <v>82.18</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>301</v>
       </c>
@@ -7909,7 +7904,7 @@
         <v>86.32</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>302</v>
       </c>
@@ -7938,7 +7933,7 @@
         <v>87.1</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>303</v>
       </c>
@@ -7967,7 +7962,7 @@
         <v>89.41</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="261" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>304</v>
       </c>
@@ -7996,7 +7991,7 @@
         <v>84.12</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>305</v>
       </c>
@@ -8025,7 +8020,7 @@
         <v>86.75</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>306</v>
       </c>
@@ -8054,7 +8049,7 @@
         <v>86.67</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>307</v>
       </c>
@@ -8083,7 +8078,7 @@
         <v>81.45</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>308</v>
       </c>
@@ -8112,7 +8107,7 @@
         <v>87.48</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="266" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>309</v>
       </c>
@@ -8141,7 +8136,7 @@
         <v>83.46</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="267" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>310</v>
       </c>
@@ -8170,7 +8165,7 @@
         <v>83.01</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="268" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>311</v>
       </c>
@@ -8199,7 +8194,7 @@
         <v>81.92</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="269" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>312</v>
       </c>
@@ -8228,7 +8223,7 @@
         <v>78.739999999999995</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="270" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>313</v>
       </c>
@@ -8257,7 +8252,7 @@
         <v>82.79</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="271" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>314</v>
       </c>
@@ -8286,7 +8281,7 @@
         <v>79.540000000000006</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>315</v>
       </c>
@@ -8315,7 +8310,7 @@
         <v>88.62</v>
       </c>
     </row>
-    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>316</v>
       </c>
@@ -8344,7 +8339,7 @@
         <v>87.36</v>
       </c>
     </row>
-    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>317</v>
       </c>
@@ -8373,7 +8368,7 @@
         <v>81.540000000000006</v>
       </c>
     </row>
-    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>318</v>
       </c>
@@ -8402,7 +8397,7 @@
         <v>82.53</v>
       </c>
     </row>
-    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>319</v>
       </c>
@@ -8431,7 +8426,7 @@
         <v>84.42</v>
       </c>
     </row>
-    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>320</v>
       </c>
@@ -8460,7 +8455,7 @@
         <v>88.03</v>
       </c>
     </row>
-    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>321</v>
       </c>
@@ -8489,7 +8484,7 @@
         <v>85.62</v>
       </c>
     </row>
-    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>322</v>
       </c>
@@ -8518,7 +8513,7 @@
         <v>87.69</v>
       </c>
     </row>
-    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>323</v>
       </c>
@@ -8547,7 +8542,7 @@
         <v>87.58</v>
       </c>
     </row>
-    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>324</v>
       </c>
@@ -8576,7 +8571,7 @@
         <v>87.44</v>
       </c>
     </row>
-    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="282" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>325</v>
       </c>
@@ -8605,7 +8600,7 @@
         <v>88.84</v>
       </c>
     </row>
-    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="283" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>326</v>
       </c>
@@ -8634,7 +8629,7 @@
         <v>88.22</v>
       </c>
     </row>
-    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>327</v>
       </c>
@@ -8663,7 +8658,7 @@
         <v>89.35</v>
       </c>
     </row>
-    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>328</v>
       </c>
@@ -8692,7 +8687,7 @@
         <v>85.14</v>
       </c>
     </row>
-    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="286" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>329</v>
       </c>
@@ -8721,7 +8716,7 @@
         <v>88.01</v>
       </c>
     </row>
-    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>330</v>
       </c>
@@ -8750,7 +8745,7 @@
         <v>89.03</v>
       </c>
     </row>
-    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="288" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>331</v>
       </c>
@@ -8779,7 +8774,7 @@
         <v>87.16</v>
       </c>
     </row>
-    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>332</v>
       </c>
@@ -8808,7 +8803,7 @@
         <v>80.73</v>
       </c>
     </row>
-    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>333</v>
       </c>
@@ -8837,7 +8832,7 @@
         <v>80.040000000000006</v>
       </c>
     </row>
-    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>334</v>
       </c>
@@ -8866,7 +8861,7 @@
         <v>80.319999999999993</v>
       </c>
     </row>
-    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>335</v>
       </c>
@@ -8895,7 +8890,7 @@
         <v>86.49</v>
       </c>
     </row>
-    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>336</v>
       </c>
@@ -8924,7 +8919,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>337</v>
       </c>
@@ -8953,7 +8948,7 @@
         <v>83.93</v>
       </c>
     </row>
-    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>338</v>
       </c>
@@ -8982,7 +8977,7 @@
         <v>88.6</v>
       </c>
     </row>
-    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>339</v>
       </c>
@@ -9011,7 +9006,7 @@
         <v>80.47</v>
       </c>
     </row>
-    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>340</v>
       </c>
@@ -9040,7 +9035,7 @@
         <v>83.84</v>
       </c>
     </row>
-    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>341</v>
       </c>
@@ -9069,7 +9064,7 @@
         <v>80.12</v>
       </c>
     </row>
-    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>342</v>
       </c>
@@ -9098,7 +9093,7 @@
         <v>89.63</v>
       </c>
     </row>
-    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>343</v>
       </c>
@@ -9127,7 +9122,7 @@
         <v>86.38</v>
       </c>
     </row>
-    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="301" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>344</v>
       </c>
@@ -9156,7 +9151,7 @@
         <v>88.91</v>
       </c>
     </row>
-    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="302" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>345</v>
       </c>
@@ -9185,7 +9180,7 @@
         <v>85.2</v>
       </c>
     </row>
-    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="303" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>346</v>
       </c>
@@ -9214,7 +9209,7 @@
         <v>83.8</v>
       </c>
     </row>
-    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="304" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>347</v>
       </c>
@@ -9243,7 +9238,7 @@
         <v>82.48</v>
       </c>
     </row>
-    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="305" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>348</v>
       </c>
@@ -9272,7 +9267,7 @@
         <v>87.39</v>
       </c>
     </row>
-    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="306" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>349</v>
       </c>
@@ -9301,7 +9296,7 @@
         <v>85.89</v>
       </c>
     </row>
-    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="307" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>350</v>
       </c>
@@ -9330,7 +9325,7 @@
         <v>87.58</v>
       </c>
     </row>
-    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="308" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>351</v>
       </c>
@@ -9359,7 +9354,7 @@
         <v>82.06</v>
       </c>
     </row>
-    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>352</v>
       </c>
@@ -9388,7 +9383,7 @@
         <v>85.41</v>
       </c>
     </row>
-    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="310" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>353</v>
       </c>
@@ -9417,7 +9412,7 @@
         <v>83.7</v>
       </c>
     </row>
-    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="311" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>354</v>
       </c>
@@ -9446,7 +9441,7 @@
         <v>81.88</v>
       </c>
     </row>
-    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="312" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>355</v>
       </c>
@@ -9475,7 +9470,7 @@
         <v>84.48</v>
       </c>
     </row>
-    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="313" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>356</v>
       </c>
@@ -9504,7 +9499,7 @@
         <v>88.76</v>
       </c>
     </row>
-    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="314" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>357</v>
       </c>
@@ -9533,7 +9528,7 @@
         <v>86.82</v>
       </c>
     </row>
-    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="315" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>358</v>
       </c>
@@ -9562,7 +9557,7 @@
         <v>86.24</v>
       </c>
     </row>
-    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="316" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>359</v>
       </c>
@@ -9591,7 +9586,7 @@
         <v>83.88</v>
       </c>
     </row>
-    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="317" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>360</v>
       </c>
@@ -9620,7 +9615,7 @@
         <v>83.97</v>
       </c>
     </row>
-    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="318" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>361</v>
       </c>
@@ -9649,7 +9644,7 @@
         <v>89.82</v>
       </c>
     </row>
-    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="319" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>362</v>
       </c>
@@ -9678,7 +9673,7 @@
         <v>83.22</v>
       </c>
     </row>
-    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="320" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>363</v>
       </c>
@@ -9707,7 +9702,7 @@
         <v>85.18</v>
       </c>
     </row>
-    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="321" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>364</v>
       </c>
@@ -9736,7 +9731,7 @@
         <v>83.72</v>
       </c>
     </row>
-    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="322" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>365</v>
       </c>
@@ -9765,7 +9760,7 @@
         <v>84.87</v>
       </c>
     </row>
-    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="323" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>366</v>
       </c>
@@ -9794,7 +9789,7 @@
         <v>89.44</v>
       </c>
     </row>
-    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="324" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>367</v>
       </c>
@@ -9823,7 +9818,7 @@
         <v>82.9</v>
       </c>
     </row>
-    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="325" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>368</v>
       </c>
@@ -9852,7 +9847,7 @@
         <v>88.94</v>
       </c>
     </row>
-    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="326" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>369</v>
       </c>
@@ -9881,7 +9876,7 @@
         <v>83.23</v>
       </c>
     </row>
-    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="327" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>370</v>
       </c>
@@ -9910,7 +9905,7 @@
         <v>74.67</v>
       </c>
     </row>
-    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="328" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>371</v>
       </c>
@@ -9939,7 +9934,7 @@
         <v>82.15</v>
       </c>
     </row>
-    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="329" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>372</v>
       </c>
@@ -9968,7 +9963,7 @@
         <v>80.5</v>
       </c>
     </row>
-    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="330" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>373</v>
       </c>
@@ -9997,7 +9992,7 @@
         <v>79.25</v>
       </c>
     </row>
-    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="331" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>374</v>
       </c>
@@ -10026,7 +10021,7 @@
         <v>87.79</v>
       </c>
     </row>
-    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="332" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>375</v>
       </c>
@@ -10036,9 +10031,6 @@
       <c r="C332">
         <v>79.11</v>
       </c>
-      <c r="D332">
-        <v>92.2</v>
-      </c>
       <c r="E332">
         <v>85.21</v>
       </c>
@@ -10055,7 +10047,7 @@
         <v>84.86</v>
       </c>
     </row>
-    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="333" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>376</v>
       </c>
@@ -10084,7 +10076,7 @@
         <v>83.06</v>
       </c>
     </row>
-    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="334" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>377</v>
       </c>
@@ -10113,7 +10105,7 @@
         <v>88.55</v>
       </c>
     </row>
-    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="335" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>378</v>
       </c>
@@ -10142,7 +10134,7 @@
         <v>84.82</v>
       </c>
     </row>
-    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="336" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>379</v>
       </c>
@@ -10171,7 +10163,7 @@
         <v>84.19</v>
       </c>
     </row>
-    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="337" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>380</v>
       </c>
@@ -10200,7 +10192,7 @@
         <v>83.69</v>
       </c>
     </row>
-    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="338" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>381</v>
       </c>
@@ -10229,7 +10221,7 @@
         <v>88.27</v>
       </c>
     </row>
-    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="339" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>382</v>
       </c>
@@ -10258,7 +10250,7 @@
         <v>86.95</v>
       </c>
     </row>
-    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="340" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>383</v>
       </c>
@@ -10316,7 +10308,7 @@
         <v>86.44</v>
       </c>
     </row>
-    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>385</v>
       </c>
@@ -10345,7 +10337,7 @@
         <v>86.24</v>
       </c>
     </row>
-    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="343" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>386</v>
       </c>
@@ -10374,7 +10366,7 @@
         <v>85.14</v>
       </c>
     </row>
-    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="344" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>387</v>
       </c>
@@ -10403,7 +10395,7 @@
         <v>88.32</v>
       </c>
     </row>
-    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="345" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>388</v>
       </c>
@@ -10432,7 +10424,7 @@
         <v>87.35</v>
       </c>
     </row>
-    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="346" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>389</v>
       </c>
@@ -10461,7 +10453,7 @@
         <v>83.21</v>
       </c>
     </row>
-    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="347" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>390</v>
       </c>
@@ -10490,7 +10482,7 @@
         <v>87.1</v>
       </c>
     </row>
-    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="348" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>391</v>
       </c>
@@ -10519,7 +10511,7 @@
         <v>89.24</v>
       </c>
     </row>
-    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="349" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>392</v>
       </c>
@@ -10548,7 +10540,7 @@
         <v>85.88</v>
       </c>
     </row>
-    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="350" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>393</v>
       </c>
@@ -10577,7 +10569,7 @@
         <v>85.64</v>
       </c>
     </row>
-    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="351" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>394</v>
       </c>
@@ -10606,7 +10598,7 @@
         <v>83.46</v>
       </c>
     </row>
-    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="352" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>395</v>
       </c>
@@ -10635,7 +10627,7 @@
         <v>88.45</v>
       </c>
     </row>
-    <row r="353" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="353" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>396</v>
       </c>
@@ -10664,7 +10656,7 @@
         <v>89.74</v>
       </c>
     </row>
-    <row r="354" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="354" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>397</v>
       </c>
@@ -10693,7 +10685,7 @@
         <v>88.12</v>
       </c>
     </row>
-    <row r="355" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>398</v>
       </c>
@@ -10722,7 +10714,7 @@
         <v>85.08</v>
       </c>
     </row>
-    <row r="356" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>399</v>
       </c>
@@ -10751,7 +10743,7 @@
         <v>87.3</v>
       </c>
     </row>
-    <row r="357" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>400</v>
       </c>
@@ -10780,7 +10772,7 @@
         <v>85.74</v>
       </c>
     </row>
-    <row r="358" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>401</v>
       </c>
@@ -10809,7 +10801,7 @@
         <v>87.2</v>
       </c>
     </row>
-    <row r="359" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>402</v>
       </c>
@@ -10838,7 +10830,7 @@
         <v>84.09</v>
       </c>
     </row>
-    <row r="360" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>403</v>
       </c>
@@ -10867,7 +10859,7 @@
         <v>87.37</v>
       </c>
     </row>
-    <row r="361" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>404</v>
       </c>
@@ -10896,7 +10888,7 @@
         <v>87.82</v>
       </c>
     </row>
-    <row r="362" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>405</v>
       </c>
@@ -10925,7 +10917,7 @@
         <v>88.78</v>
       </c>
     </row>
-    <row r="363" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>406</v>
       </c>
@@ -10954,7 +10946,7 @@
         <v>80.010000000000005</v>
       </c>
     </row>
-    <row r="364" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>407</v>
       </c>
@@ -10983,7 +10975,7 @@
         <v>80.150000000000006</v>
       </c>
     </row>
-    <row r="365" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>408</v>
       </c>
@@ -11012,7 +11004,7 @@
         <v>85.13</v>
       </c>
     </row>
-    <row r="366" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>409</v>
       </c>
@@ -11041,7 +11033,7 @@
         <v>83.27</v>
       </c>
     </row>
-    <row r="367" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>410</v>
       </c>
@@ -11070,7 +11062,7 @@
         <v>88.4</v>
       </c>
     </row>
-    <row r="368" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>411</v>
       </c>
@@ -11099,7 +11091,7 @@
         <v>80.06</v>
       </c>
     </row>
-    <row r="369" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>412</v>
       </c>
@@ -11128,7 +11120,7 @@
         <v>82.37</v>
       </c>
     </row>
-    <row r="370" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>413</v>
       </c>
@@ -11157,7 +11149,7 @@
         <v>85.48</v>
       </c>
     </row>
-    <row r="371" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>414</v>
       </c>
@@ -11186,7 +11178,7 @@
         <v>86.96</v>
       </c>
     </row>
-    <row r="372" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>415</v>
       </c>
@@ -11215,7 +11207,7 @@
         <v>86.32</v>
       </c>
     </row>
-    <row r="373" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>416</v>
       </c>
@@ -11244,7 +11236,7 @@
         <v>82.88</v>
       </c>
     </row>
-    <row r="374" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>417</v>
       </c>
@@ -11273,7 +11265,7 @@
         <v>84.45</v>
       </c>
     </row>
-    <row r="375" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>418</v>
       </c>
@@ -11302,7 +11294,7 @@
         <v>84.69</v>
       </c>
     </row>
-    <row r="376" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>419</v>
       </c>
@@ -11331,7 +11323,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="377" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>420</v>
       </c>
@@ -11360,7 +11352,7 @@
         <v>89.29</v>
       </c>
     </row>
-    <row r="378" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>421</v>
       </c>
@@ -11389,7 +11381,7 @@
         <v>78.099999999999994</v>
       </c>
     </row>
-    <row r="379" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>422</v>
       </c>
@@ -11418,7 +11410,7 @@
         <v>84.38</v>
       </c>
     </row>
-    <row r="380" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="380" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>423</v>
       </c>
@@ -11447,7 +11439,7 @@
         <v>81.36</v>
       </c>
     </row>
-    <row r="381" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="381" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>424</v>
       </c>
@@ -11477,6 +11469,16 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:J381">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="184"/>
+        <filter val="284"/>
+        <filter val="384"/>
+        <filter val="84"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>